<commit_message>
V0.2.0 - Modifiche Ragazzi
</commit_message>
<xml_diff>
--- a/CarbonFootprint_site/results_download.xlsx
+++ b/CarbonFootprint_site/results_download.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tables" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tables" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -234,14 +234,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -264,8 +264,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -279,7 +279,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -287,71 +287,71 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
             <strRef>
-              <f>Tables!$C$4:$C$7</f>
+              <f>Tables!$C$4:$C$9</f>
               <strCache>
-                <ptCount val="4"/>
+                <ptCount val="6"/>
                 <pt idx="0">
                   <v>Wheat &amp; Rye</v>
                 </pt>
@@ -363,27 +363,39 @@
                 </pt>
                 <pt idx="3">
                   <v>Cane sugar</v>
+                </pt>
+                <pt idx="4">
+                  <v>Pasta</v>
+                </pt>
+                <pt idx="5">
+                  <v>Bread</v>
                 </pt>
               </strCache>
             </strRef>
           </cat>
           <val>
             <numRef>
-              <f>Tables!$D$4:$D$7</f>
+              <f>Tables!$D$4:$D$9</f>
               <numCache>
                 <formatCode>General</formatCode>
-                <ptCount val="4"/>
+                <ptCount val="6"/>
                 <pt idx="0">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.0005714285714285714</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>0</v>
+                  <v>#N/A</v>
+                </pt>
+                <pt idx="4">
+                  <v>#N/A</v>
+                </pt>
+                <pt idx="5">
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -404,16 +416,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -437,33 +449,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -486,8 +483,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -501,7 +498,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -509,96 +506,96 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -634,22 +631,22 @@
                 <formatCode>General</formatCode>
                 <ptCount val="6"/>
                 <pt idx="0">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1838356164383562</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="4">
-                  <v>1.118082191780822</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="5">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -670,16 +667,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -703,33 +700,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -752,8 +734,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -767,7 +749,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -775,64 +757,64 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -862,16 +844,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0.04828571428571428</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.1228512720156556</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>1.301917808219178</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>1.41778</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -892,16 +874,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -925,33 +907,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -974,8 +941,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -989,7 +956,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -997,168 +964,168 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="6"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="7"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="8"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="9"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -1206,34 +1173,34 @@
                 <formatCode>General</formatCode>
                 <ptCount val="10"/>
                 <pt idx="0">
-                  <v>0.04285714285714286</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="4">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="5">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="6">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="7">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="8">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="9">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1254,16 +1221,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1287,33 +1254,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1336,8 +1288,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1351,7 +1303,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -1359,242 +1311,242 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="6"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="7"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="8"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="9"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="10"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent5">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="11"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent6">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="12"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="13"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -1654,46 +1606,46 @@
                 <formatCode>General</formatCode>
                 <ptCount val="14"/>
                 <pt idx="0">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="4">
-                  <v>0.0005714285714285714</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="5">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="6">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="7">
-                  <v>0.004285714285714285</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="8">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="9">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="10">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="11">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="12">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="13">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1714,16 +1666,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1747,33 +1699,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1796,8 +1733,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1811,7 +1748,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -1819,48 +1756,48 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -1887,13 +1824,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>0.004857142857142857</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.0005714285714285714</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.04285714285714286</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -1914,16 +1851,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1947,33 +1884,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1996,8 +1918,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2011,7 +1933,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2019,48 +1941,48 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2087,13 +2009,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>0.002136986301369863</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.09142857142857144</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0.02928571428571429</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2114,16 +2036,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2147,33 +2069,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2201,8 +2108,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2216,7 +2123,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2224,64 +2131,64 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2311,16 +2218,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.02928571428571429</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2341,16 +2248,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2374,33 +2281,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2423,8 +2315,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2438,7 +2330,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2446,64 +2338,64 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2533,16 +2425,16 @@
                 <formatCode>General</formatCode>
                 <ptCount val="4"/>
                 <pt idx="0">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.09142857142857144</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2563,16 +2455,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2596,33 +2488,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2645,8 +2522,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2660,7 +2537,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2668,48 +2545,48 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2736,13 +2613,13 @@
                 <formatCode>General</formatCode>
                 <ptCount val="3"/>
                 <pt idx="0">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.002136986301369863</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -2763,16 +2640,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2796,33 +2673,18 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2845,8 +2707,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2860,7 +2722,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2868,139 +2730,139 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="6"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="7"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill>
+              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d contourW="25400"/>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
             <strRef>
-              <f>Tables!$A$37:$A$44</f>
+              <f>Tables!$A$37:$A$45</f>
               <strCache>
-                <ptCount val="8"/>
+                <ptCount val="9"/>
                 <pt idx="0">
                   <v>Refrigerator</v>
                 </pt>
@@ -3024,39 +2886,45 @@
                 </pt>
                 <pt idx="7">
                   <v>Heating</v>
+                </pt>
+                <pt idx="8">
+                  <v>Cooling</v>
                 </pt>
               </strCache>
             </strRef>
           </cat>
           <val>
             <numRef>
-              <f>Tables!$B$37:$B$44</f>
+              <f>Tables!$B$37:$B$45</f>
               <numCache>
                 <formatCode>General</formatCode>
-                <ptCount val="8"/>
+                <ptCount val="9"/>
                 <pt idx="0">
-                  <v>0.14</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="1">
-                  <v>0.05048</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="2">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="3">
-                  <v>0.6283</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="4">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="5">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="6">
-                  <v>0</v>
+                  <v>#N/A</v>
                 </pt>
                 <pt idx="7">
-                  <v>0.5990000000000001</v>
+                  <v>#N/A</v>
+                </pt>
+                <pt idx="8">
+                  <v>#N/A</v>
                 </pt>
               </numCache>
             </numRef>
@@ -3077,16 +2945,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill/>
-        <a:ln>
+        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -3110,26 +2978,11 @@
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
-  <spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:prstDash val="solid"/>
-      <a:round/>
-    </a:ln>
-  </spPr>
 </chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>8</col>
@@ -3149,9 +3002,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3176,9 +3029,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3203,9 +3056,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3230,9 +3083,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3257,9 +3110,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3284,9 +3137,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId6"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3311,9 +3164,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId7"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3338,9 +3191,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId8"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3365,9 +3218,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId9"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3392,9 +3245,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId10"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3419,9 +3272,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId11"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3699,20 +3552,20 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="31.85546875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="15.7109375" customWidth="1" min="2" max="2"/>
-    <col width="28.140625" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="25.7109375" customWidth="1" min="4" max="4"/>
-    <col width="31.85546875" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="15.7109375" customWidth="1" min="6" max="6"/>
-    <col width="13.140625" customWidth="1" min="7" max="7"/>
-    <col width="30.28515625" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="31.88671875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="15.77734375" customWidth="1" min="2" max="2"/>
+    <col width="28.109375" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="25.77734375" customWidth="1" min="4" max="4"/>
+    <col width="31.88671875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="15.77734375" customWidth="1" min="6" max="6"/>
+    <col width="13.109375" customWidth="1" min="7" max="7"/>
+    <col width="30.21875" bestFit="1" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3791,7 +3644,7 @@
         </is>
       </c>
       <c r="B4" s="4">
-        <f>SUMIF(Sheet3!A:A, "beef_herd", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("beef_herd",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -3800,7 +3653,7 @@
         </is>
       </c>
       <c r="D4" s="4">
-        <f>SUMIF(Sheet3!A:A, "wheat_rye", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("wheat_rye",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E4" s="2" t="inlineStr">
@@ -3809,7 +3662,7 @@
         </is>
       </c>
       <c r="F4" s="4">
-        <f>SUMIF(Sheet3!A:A, "apples", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("apples",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3820,7 +3673,7 @@
         </is>
       </c>
       <c r="B5" s="4">
-        <f>SUMIF(Sheet3!A:A, "lumb_mutton", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("lumb_mutton",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C5" s="2" t="inlineStr">
@@ -3829,7 +3682,7 @@
         </is>
       </c>
       <c r="D5" s="4">
-        <f>SUMIF(Sheet3!A:A, "maize",  Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("maize",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E5" s="2" t="inlineStr">
@@ -3838,7 +3691,7 @@
         </is>
       </c>
       <c r="F5" s="4">
-        <f>SUMIF(Sheet3!A:A, "chocolate", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("chocolate",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3849,7 +3702,7 @@
         </is>
       </c>
       <c r="B6" s="4">
-        <f>SUMIF(Sheet3!A:A, "cheese", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("cheese",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C6" s="2" t="inlineStr">
@@ -3858,7 +3711,7 @@
         </is>
       </c>
       <c r="D6" s="4">
-        <f>SUMIF(Sheet3!A:A, "rice", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("rice",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E6" s="2" t="inlineStr">
@@ -3867,7 +3720,7 @@
         </is>
       </c>
       <c r="F6" s="4">
-        <f>SUMIF(Sheet3!A:A, "coffee", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("coffee",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3878,7 +3731,7 @@
         </is>
       </c>
       <c r="B7" s="4">
-        <f>SUMIF(Sheet3!A:A, "beef_dairy", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("beef_dairy",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C7" s="2" t="inlineStr">
@@ -3887,7 +3740,7 @@
         </is>
       </c>
       <c r="D7" s="4">
-        <f>SUMIF(Sheet3!A:A, "cane_sugar", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("cane_sugar",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E7" s="2" t="inlineStr">
@@ -3896,7 +3749,7 @@
         </is>
       </c>
       <c r="F7" s="4">
-        <f>SUMIF(Sheet3!A:A, "tomatoes", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("tomatoes",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3907,18 +3760,25 @@
         </is>
       </c>
       <c r="B8" s="4">
-        <f>SUMIF(Sheet3!A:A, "poultry_meat", Sheet3!B:B)</f>
-        <v/>
-      </c>
-      <c r="C8" s="2" t="n"/>
-      <c r="D8" s="4" t="n"/>
+        <f>_xlfn.XLOOKUP("poultry_meat",Sheet3!A:A,Sheet3!B:B)</f>
+        <v/>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Pasta</t>
+        </is>
+      </c>
+      <c r="D8" s="4">
+        <f>_xlfn.XLOOKUP("pasta",Sheet3!A:A,Sheet3!B:B)</f>
+        <v/>
+      </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
           <t>Maize (corn)</t>
         </is>
       </c>
       <c r="F8" s="4">
-        <f>SUMIF(Sheet3!A:A, "maize", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("maize",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3929,18 +3789,25 @@
         </is>
       </c>
       <c r="B9" s="4">
-        <f>SUMIF(Sheet3!A:A, "pig_meat", Sheet3!B:B)</f>
-        <v/>
-      </c>
-      <c r="C9" s="2" t="n"/>
-      <c r="D9" s="4" t="n"/>
+        <f>_xlfn.XLOOKUP("pig_meat",Sheet3!A:A,Sheet3!B:B)</f>
+        <v/>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Bread</t>
+        </is>
+      </c>
+      <c r="D9" s="4">
+        <f>_xlfn.XLOOKUP("bread",Sheet3!A:A,Sheet3!B:B)</f>
+        <v/>
+      </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
           <t>Peas</t>
         </is>
       </c>
       <c r="F9" s="4">
-        <f>SUMIF(Sheet3!A:A, "peas", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("peas",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3951,7 +3818,7 @@
         </is>
       </c>
       <c r="B10" s="4">
-        <f>SUMIF(Sheet3!A:A, "prawns_farmed", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("prawns_farmed",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C10" s="2" t="n"/>
@@ -3962,7 +3829,7 @@
         </is>
       </c>
       <c r="F10" s="4">
-        <f>SUMIF(Sheet3!A:A, "soy_milk", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("soy_milk",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3973,7 +3840,7 @@
         </is>
       </c>
       <c r="B11" s="4">
-        <f>SUMIF(Sheet3!A:A, "fish_farmed", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("fish_farmed",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C11" s="2" t="n"/>
@@ -3984,7 +3851,7 @@
         </is>
       </c>
       <c r="F11" s="4">
-        <f>SUMIF(Sheet3!A:A, "olive_oil", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("olive_oil",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -3995,7 +3862,7 @@
         </is>
       </c>
       <c r="B12" s="4">
-        <f>SUMIF(Sheet3!A:A, "fish_wildcatch", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("fish_wildcatch",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C12" s="2" t="n"/>
@@ -4006,7 +3873,7 @@
         </is>
       </c>
       <c r="F12" s="4">
-        <f>SUMIF(Sheet3!A:A, "milk", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("milk",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4017,7 +3884,7 @@
         </is>
       </c>
       <c r="B13" s="4">
-        <f>SUMIF(Sheet3!A:A, "eggs", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("eggs",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C13" s="2" t="n"/>
@@ -4028,7 +3895,7 @@
         </is>
       </c>
       <c r="F13" s="4">
-        <f>SUMIF(Sheet3!A:A, "groundnuts", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("groundnuts",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4043,7 +3910,7 @@
         </is>
       </c>
       <c r="F14" s="4">
-        <f>SUMIF(Sheet3!A:A, "bananas", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("bananas",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4058,7 +3925,7 @@
         </is>
       </c>
       <c r="F15" s="4">
-        <f>SUMIF(Sheet3!A:A, "root_vegetables", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("root_vegetables",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4073,7 +3940,7 @@
         </is>
       </c>
       <c r="F16" s="4">
-        <f>SUMIF(Sheet3!A:A, "citrus_fruit", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("citrus_fruit",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4088,7 +3955,7 @@
         </is>
       </c>
       <c r="F17" s="4">
-        <f>SUMIF(Sheet3!A:A, "nuts", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("nuts",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4124,7 +3991,7 @@
         </is>
       </c>
       <c r="B20">
-        <f>SUM(D4:D7)</f>
+        <f>SUM(D4:D9)</f>
         <v/>
       </c>
       <c r="C20" t="inlineStr">
@@ -4238,7 +4105,7 @@
         </is>
       </c>
       <c r="B26" s="4">
-        <f>SUMIF(Sheet3!A:A, "bus", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("bus",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C26" s="2" t="inlineStr">
@@ -4247,7 +4114,7 @@
         </is>
       </c>
       <c r="D26" s="4">
-        <f>SUMIF(Sheet3!A:A,"mediumcar_petrol",Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("mediumcar_petrol",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E26" s="2" t="inlineStr">
@@ -4256,7 +4123,7 @@
         </is>
       </c>
       <c r="F26" s="4">
-        <f>SUMIF(Sheet3!A:A,"domestic_flight",Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("domestic_flight",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4267,7 +4134,7 @@
         </is>
       </c>
       <c r="B27" s="4">
-        <f>SUMIF(Sheet3!A:A, "national_rail", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("national_rail",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C27" s="2" t="inlineStr">
@@ -4276,7 +4143,7 @@
         </is>
       </c>
       <c r="D27" s="4">
-        <f>SUMIF(Sheet3!A:A,"mediumcar_diesel", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("mediumcar_diesel",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E27" s="2" t="inlineStr">
@@ -4285,7 +4152,7 @@
         </is>
       </c>
       <c r="F27" s="4">
-        <f>SUMIF(Sheet3!A:A,"short_flight", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("short_flight",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4296,7 +4163,7 @@
         </is>
       </c>
       <c r="B28" s="4">
-        <f>SUMIF(Sheet3!A:A, "ferry", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("ferry",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C28" s="2" t="inlineStr">
@@ -4305,7 +4172,7 @@
         </is>
       </c>
       <c r="D28" s="4">
-        <f>SUMIF(Sheet3!A:A,"motorcycle", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("motorcycle",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E28" s="2" t="inlineStr">
@@ -4314,7 +4181,7 @@
         </is>
       </c>
       <c r="F28" s="4">
-        <f>SUMIF(Sheet3!A:A, "long_flight", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("long_flight",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4325,7 +4192,7 @@
         </is>
       </c>
       <c r="B29" s="4">
-        <f>SUMIF(Sheet3!A:A, "eurostar", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("eurostar",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="C29" s="2" t="inlineStr">
@@ -4334,7 +4201,7 @@
         </is>
       </c>
       <c r="D29" s="4">
-        <f>SUMIF(Sheet3!A:A, "electric_vehicle", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("electric_vehicle",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="E29" s="2" t="n"/>
@@ -4460,7 +4327,7 @@
         </is>
       </c>
       <c r="B37" s="4">
-        <f>SUMIF(Sheet3!A:A, "refrigerator", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("refrigerator",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="D37" s="2" t="inlineStr">
@@ -4469,7 +4336,7 @@
         </is>
       </c>
       <c r="E37" s="4">
-        <f>SUMIF(Sheet3!A:A, "cotton_shirt", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("cotton_shirt",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4480,7 +4347,7 @@
         </is>
       </c>
       <c r="B38" s="4">
-        <f>SUMIF(Sheet3!A:A, "food_cooking", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("food_cooking",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="D38" s="2" t="inlineStr">
@@ -4489,7 +4356,7 @@
         </is>
       </c>
       <c r="E38" s="4">
-        <f>SUMIF(Sheet3!A:A, "cotton_sweatjacket", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("cotton_sweatjacket",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4500,7 +4367,7 @@
         </is>
       </c>
       <c r="B39" s="4">
-        <f>SUMIF(Sheet3!A:A, "oven", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("oven",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="D39" s="2" t="inlineStr">
@@ -4509,7 +4376,7 @@
         </is>
       </c>
       <c r="E39" s="4">
-        <f>SUMIF(Sheet3!A:A, "acrylic_jacket", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("acrylic_jacket",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4520,7 +4387,7 @@
         </is>
       </c>
       <c r="B40" s="4">
-        <f>SUMIF(Sheet3!A:A, "washing_machine", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("washing_machine",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -4529,7 +4396,7 @@
         </is>
       </c>
       <c r="E40" s="4">
-        <f>SUMIF(Sheet3!A:A, "woolen_sweater", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("woolen_sweater",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4540,7 +4407,7 @@
         </is>
       </c>
       <c r="B41" s="4">
-        <f>SUMIF(Sheet3!A:A, "personal_cleaning", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("shower",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="D41" s="2" t="inlineStr">
@@ -4549,7 +4416,7 @@
         </is>
       </c>
       <c r="E41" s="4">
-        <f>SUMIF(Sheet3!A:A, "polyester_shirt", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("polyester_shirt",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4560,7 +4427,7 @@
         </is>
       </c>
       <c r="B42" s="4">
-        <f>SUMIF(Sheet3!A:A, "laptop", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("laptop",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
       <c r="D42" s="2" t="inlineStr">
@@ -4569,7 +4436,7 @@
         </is>
       </c>
       <c r="E42" s="4">
-        <f>SUMIF(Sheet3!A:A, "jeans", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("jeans",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4580,7 +4447,7 @@
         </is>
       </c>
       <c r="B43" s="4">
-        <f>SUMIF(Sheet3!A:A, "smartphone", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("smartphone",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4591,7 +4458,18 @@
         </is>
       </c>
       <c r="B44" s="4">
-        <f>SUMIF(Sheet3!A:A, "heating", Sheet3!B:B)</f>
+        <f>_xlfn.XLOOKUP("heating",Sheet3!A:A,Sheet3!B:B)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="inlineStr">
+        <is>
+          <t>Cooling</t>
+        </is>
+      </c>
+      <c r="B45" s="4">
+        <f>_xlfn.XLOOKUP("cooling",Sheet3!A:A,Sheet3!B:B)</f>
         <v/>
       </c>
     </row>
@@ -4602,7 +4480,7 @@
         </is>
       </c>
       <c r="B46">
-        <f>SUM(B4:B13,D4:D7,F4:F17)</f>
+        <f>SUM(B4:B13,D4:D9,F4:F17)</f>
         <v/>
       </c>
       <c r="C46" t="inlineStr">
@@ -4677,7 +4555,7 @@
         </is>
       </c>
       <c r="B49">
-        <f>SUM(B37:B44)</f>
+        <f>SUM(B37:B45)</f>
         <v/>
       </c>
       <c r="C49" t="inlineStr">
@@ -4722,16 +4600,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A2:B2"/>
     <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C2:D2"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A35:B35"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -4739,21 +4617,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView topLeftCell="D67" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4763,15 +4641,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="18.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="12" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4781,7 +4659,7 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>0.008571428571428572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -4791,7 +4669,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.003428571428571428</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -4801,7 +4679,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -4811,7 +4689,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -4821,7 +4699,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.02985714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -4831,7 +4709,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.05953</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -4841,7 +4719,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.001714285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -4851,7 +4729,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -4861,7 +4739,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -4871,7 +4749,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -4881,7 +4759,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0001428571428571428</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -4891,7 +4769,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.0001285714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -4901,7 +4779,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0001285714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -4911,7 +4789,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.0008571428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -4921,7 +4799,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.0008571428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -4931,7 +4809,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.0007142857142857143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -4941,7 +4819,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.0002714285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -4951,7 +4829,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.0001044285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -4961,7 +4839,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.03214285714285715</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -4971,7 +4849,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.0005714285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -4981,7 +4859,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.0004285714285714285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -4991,7 +4869,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.0004285714285714285</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -5001,7 +4879,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.004714285714285714</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -5011,7 +4889,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.003928571428571429</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -5031,7 +4909,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.0006285714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -5051,7 +4929,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.01071428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -5061,7 +4939,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>4.285714285714286e-05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -5071,7 +4949,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.0006986301369863014</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -5081,7 +4959,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.02742857142857143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -5091,7 +4969,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0.2687142857142857</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -5101,7 +4979,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0.004701369863013699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -5111,7 +4989,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>0.000410958904109589</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -5121,7 +4999,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -5131,7 +5009,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>0.01471428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -5141,7 +5019,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.01828571428571429</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="38">
@@ -5151,7 +5029,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0.005857142857142858</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -5161,7 +5039,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>0.02985714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -5171,7 +5049,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>0.0008571428571428572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -5181,7 +5059,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0.14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -5191,7 +5069,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0.55528</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -5201,7 +5079,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0.7091</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -5211,17 +5089,17 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0.6283</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>personal_cleaning</t>
+          <t>shower</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>0.6057</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -5231,7 +5109,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0.273972602739726</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -5241,7 +5119,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>0.3287671232876712</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -5251,67 +5129,77 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>2.995</v>
+        <v>0.007808219178082192</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>cotton_shirt</t>
+          <t>cooling</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.02945205479452055</v>
+        <v>0.0007136986301369863</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>cotton_sweatjacket</t>
+          <t>cotton_shirt</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.03676712328767123</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>acrylic_jacket</t>
+          <t>cotton_sweatjacket</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>0.411972602739726</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>woolen_sweater</t>
+          <t>acrylic_jacket</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>0.03594520547945206</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>polyester_shirt</t>
+          <t>woolen_sweater</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>24.82142465753425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>polyester_shirt</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>jeans</t>
         </is>
       </c>
-      <c r="B54" t="n">
-        <v>0.2475890410958904</v>
+      <c r="B55" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
V0.3.0 - HTML Rewritten
</commit_message>
<xml_diff>
--- a/CarbonFootprint_site/results_download.xlsx
+++ b/CarbonFootprint_site/results_download.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tables" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Tables" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -234,14 +234,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -264,8 +264,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -279,7 +279,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -287,64 +287,64 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -416,16 +416,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -453,14 +453,14 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -483,8 +483,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -498,7 +498,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -506,96 +506,96 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -667,16 +667,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -704,14 +704,14 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -734,8 +734,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -749,7 +749,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -757,64 +757,64 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -874,16 +874,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -911,14 +911,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -941,8 +941,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -956,7 +956,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -964,168 +964,168 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="6"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="7"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="8"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="9"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -1221,16 +1221,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1258,14 +1258,14 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1288,8 +1288,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1303,7 +1303,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -1311,242 +1311,242 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="6"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="7"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="8"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="9"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="10"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent5">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="11"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent6">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="12"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="13"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="80000"/>
                   <a:lumOff val="20000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -1666,16 +1666,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1703,14 +1703,14 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1733,8 +1733,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1748,7 +1748,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -1756,48 +1756,48 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -1851,16 +1851,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -1888,14 +1888,14 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -1918,8 +1918,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -1933,7 +1933,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -1941,48 +1941,48 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2036,16 +2036,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2073,14 +2073,14 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2108,8 +2108,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2123,7 +2123,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2131,64 +2131,64 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2248,16 +2248,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2285,14 +2285,14 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2315,8 +2315,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2330,7 +2330,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2338,64 +2338,64 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2455,16 +2455,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2492,14 +2492,14 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2522,8 +2522,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2537,7 +2537,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2545,48 +2545,48 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2640,16 +2640,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2677,14 +2677,14 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
             <a:pPr>
               <a:defRPr sz="1400" b="0" i="0" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
@@ -2707,8 +2707,8 @@
       </tx>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -2722,7 +2722,7 @@
           <idx val="0"/>
           <order val="0"/>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
@@ -2730,132 +2730,132 @@
             <idx val="0"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="1"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="2"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="3"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="4"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="5"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="6"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <dPt>
             <idx val="7"/>
             <bubble3D val="0"/>
             <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:solidFill>
                 <a:schemeClr val="accent2">
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="lt1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-              <a:sp3d xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" contourW="25400"/>
+              <a:ln w="25400">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:sp3d contourW="25400"/>
             </spPr>
           </dPt>
           <cat>
@@ -2945,16 +2945,16 @@
       <legendPos val="b"/>
       <overlay val="0"/>
       <spPr>
-        <a:noFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
           <a:prstDash val="solid"/>
         </a:ln>
       </spPr>
       <txPr>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
@@ -2982,7 +2982,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>8</col>
@@ -3002,9 +3002,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3029,9 +3029,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3056,9 +3056,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3083,9 +3083,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3110,9 +3110,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3137,9 +3137,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+          <c:chart r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3164,9 +3164,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+          <c:chart r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3191,9 +3191,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+          <c:chart r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3218,9 +3218,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+          <c:chart r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3245,9 +3245,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+          <c:chart r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -3272,9 +3272,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+          <c:chart r:id="rId11"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -4600,16 +4600,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E2:F2"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="A23:F23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="D35:E35"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -4617,7 +4617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -4631,7 +4631,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5019,7 +5019,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -5129,7 +5129,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>0.007808219178082192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -5139,7 +5139,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>0.0007136986301369863</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">

</xml_diff>